<commit_message>
Add User Data To AspnetUsers
</commit_message>
<xml_diff>
--- a/DigiMovie/INFOs/Permissions.xlsx
+++ b/DigiMovie/INFOs/Permissions.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92ED443F-79FD-432F-8139-285A787D42A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
   <si>
     <t>Products</t>
   </si>
@@ -133,12 +134,15 @@
   </si>
   <si>
     <t>_ManagementPartial &gt; check in view for menu items</t>
+  </si>
+  <si>
+    <t>_LoginPartial &gt; check in view for menu item</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -312,74 +316,74 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,27 +670,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="57.5703125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="1"/>
-    <col min="12" max="14" width="9.140625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.109375" style="1"/>
+    <col min="9" max="9" width="57.5546875" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.109375" style="1"/>
+    <col min="12" max="14" width="9.109375" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -703,8 +707,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -713,33 +717,36 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="I2" s="30" t="s">
+      <c r="D2" s="22"/>
+      <c r="I2" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="15"/>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="D3" s="23"/>
+      <c r="I3" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="D4" s="24"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -752,8 +759,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -762,8 +769,8 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -774,40 +781,40 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="16" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+      <c r="D9" s="17"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="D10" s="18"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -820,8 +827,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
+    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="29"/>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
@@ -830,8 +837,8 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
+    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="29"/>
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
@@ -842,8 +849,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
+    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="29"/>
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
@@ -852,40 +859,40 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="29"/>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="28" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="21"/>
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="29"/>
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="21"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
+      <c r="D16" s="29"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="30"/>
       <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="22"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="19" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -894,42 +901,42 @@
       <c r="C18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="20"/>
       <c r="B19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="9"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="D19" s="20"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="20"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="9"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="10"/>
+      <c r="D20" s="20"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
       <c r="B21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="11" t="s">
+      <c r="D21" s="21"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="25" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -938,139 +945,139 @@
       <c r="C22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="26"/>
       <c r="B23" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="12"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
+      <c r="D23" s="26"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="26"/>
       <c r="B24" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="12"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
+      <c r="D24" s="26"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="26"/>
       <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="12"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="26"/>
       <c r="B26" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="12"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="26"/>
       <c r="B27" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="12"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="12"/>
+      <c r="D27" s="26"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="26"/>
       <c r="B28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="12"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="26"/>
       <c r="B29" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="12"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="13"/>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="27"/>
       <c r="B30" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="13"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
+      <c r="D30" s="27"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="23" t="s">
+      <c r="B31" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C31" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="27" t="s">
+      <c r="C31" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="24"/>
-      <c r="B32" s="23" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="12"/>
+      <c r="B32" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C32" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="28"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="24"/>
-      <c r="B33" s="23" t="s">
+      <c r="C32" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" s="14"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="12"/>
+      <c r="B33" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C33" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="28"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="24"/>
-      <c r="B34" s="23" t="s">
+      <c r="C33" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" s="14"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
+      <c r="B34" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="29"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="26"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="26"/>
+      <c r="C34" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="15"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C35" s="10"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C36" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Edit Excel Of Permissions
</commit_message>
<xml_diff>
--- a/DigiMovie/INFOs/Permissions.xlsx
+++ b/DigiMovie/INFOs/Permissions.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92ED443F-79FD-432F-8139-285A787D42A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
   <si>
     <t>Products</t>
   </si>
@@ -137,13 +136,16 @@
   </si>
   <si>
     <t>_LoginPartial &gt; check in view for menu item</t>
+  </si>
+  <si>
+    <t>Users</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,14 +168,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -225,6 +221,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF996633"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF66"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,9 +324,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -384,6 +383,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -393,6 +398,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF99FF66"/>
       <color rgb="FF996633"/>
       <color rgb="FFFF99FF"/>
     </mruColors>
@@ -670,27 +676,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.109375" style="1"/>
-    <col min="9" max="9" width="57.5546875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.109375" style="1"/>
-    <col min="12" max="14" width="9.109375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.109375" style="1"/>
+    <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="57.5703125" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="1"/>
+    <col min="12" max="14" width="9.140625" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -707,8 +713,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -717,36 +723,36 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="I2" s="11" t="s">
+      <c r="D2" s="21"/>
+      <c r="I2" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="I3" s="11" t="s">
+      <c r="D3" s="22"/>
+      <c r="I3" s="10" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="24"/>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="24"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -759,8 +765,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="17"/>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -769,8 +775,8 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="17"/>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
@@ -781,40 +787,40 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="17"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="18"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="17"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="18"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="28" t="s">
+      <c r="D10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -827,8 +833,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="29"/>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="28"/>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
@@ -837,8 +843,8 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="29"/>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
@@ -849,8 +855,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="29"/>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
@@ -859,40 +865,40 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="29"/>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="28" t="s">
+      <c r="D15" s="27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="29"/>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="29"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="30"/>
+      <c r="D16" s="28"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="29"/>
       <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="30"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="19" t="s">
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -901,42 +907,42 @@
       <c r="C18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="20"/>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="19"/>
       <c r="B19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="20"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="20"/>
+      <c r="D19" s="19"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="19"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="20"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
       <c r="B21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="21"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="25" t="s">
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -945,92 +951,92 @@
       <c r="C22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="24" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="26"/>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="25"/>
       <c r="B23" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="26"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="26"/>
+      <c r="D23" s="25"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="25"/>
       <c r="B24" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="26"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="26"/>
+      <c r="D24" s="25"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
       <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="26"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="26"/>
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
       <c r="B26" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="26"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="26"/>
+      <c r="D26" s="25"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
       <c r="B27" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="26"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="26"/>
+      <c r="D27" s="25"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
       <c r="B28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="26"/>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
       <c r="B29" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="26"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="27"/>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="26"/>
       <c r="B30" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="27"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="12" t="s">
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -1039,48 +1045,88 @@
       <c r="C31" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D31" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
       <c r="B32" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="14"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="12"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
       <c r="B33" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="14"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="12"/>
+      <c r="D33" s="13"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="11"/>
       <c r="B34" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D34" s="15"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C35" s="10"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C36" s="10"/>
+      <c r="D34" s="14"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" s="30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="30"/>
+      <c r="B36" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" s="30"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="30"/>
+      <c r="B37" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="30"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="30"/>
+      <c r="B38" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D38" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="A35:A38"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="D31:D34"/>
     <mergeCell ref="A5:A10"/>

</xml_diff>

<commit_message>
Add Authorization To Site
</commit_message>
<xml_diff>
--- a/DigiMovie/INFOs/Permissions.xlsx
+++ b/DigiMovie/INFOs/Permissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
   <si>
     <t>Products</t>
   </si>
@@ -148,6 +148,36 @@
   </si>
   <si>
     <t>AddUserToRole</t>
+  </si>
+  <si>
+    <t>admin@admin.ir</t>
+  </si>
+  <si>
+    <t>مدیر محصولات</t>
+  </si>
+  <si>
+    <t>مدیر دسته بندی ها</t>
+  </si>
+  <si>
+    <t>مدیر پیام ها</t>
+  </si>
+  <si>
+    <t>qwQW12!@</t>
+  </si>
+  <si>
+    <t>Annonymous / مدیر محصولات</t>
+  </si>
+  <si>
+    <t>Annonymous / مدیر دسته بندی ها</t>
+  </si>
+  <si>
+    <t>مدیر عضویت</t>
+  </si>
+  <si>
+    <t>Admin User</t>
+  </si>
+  <si>
+    <t>[has all roles]</t>
   </si>
 </sst>
 </file>
@@ -178,7 +208,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -242,6 +272,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -310,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -345,6 +387,60 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -360,56 +456,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -698,26 +746,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="57.5703125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="1"/>
-    <col min="12" max="14" width="9.140625" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="5" max="5" width="2.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17" style="1" customWidth="1"/>
+    <col min="9" max="9" width="2" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5703125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="1"/>
+    <col min="13" max="15" width="9.140625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -730,12 +782,18 @@
       <c r="D1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="H1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -744,50 +802,71 @@
       <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="I2" s="10" t="s">
+      <c r="D2" s="18"/>
+      <c r="F2" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
+      <c r="H2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="J2" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="I3" s="10" t="s">
+      <c r="D3" s="19"/>
+      <c r="F3" s="10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
+      <c r="H3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="25"/>
-    </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="D4" s="20"/>
+      <c r="H4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="35" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="H5" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="28"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
@@ -796,66 +875,66 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="28"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+    <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="28"/>
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="28"/>
       <c r="B9" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="18"/>
-    </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
+        <v>44</v>
+      </c>
+      <c r="D9" s="28"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="29"/>
       <c r="B10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="19"/>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="29"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="25"/>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
@@ -864,20 +943,20 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
       <c r="B13" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
@@ -886,84 +965,84 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
       <c r="B15" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D15" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
       <c r="B16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="30"/>
+        <v>45</v>
+      </c>
+      <c r="D16" s="25"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
+      <c r="A17" s="26"/>
       <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="31"/>
+        <v>45</v>
+      </c>
+      <c r="D17" s="26"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="14" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D18" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="14" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D19" s="21"/>
+        <v>46</v>
+      </c>
+      <c r="D19" s="15"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="21"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D20" s="21"/>
+        <v>46</v>
+      </c>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="22"/>
+        <v>46</v>
+      </c>
+      <c r="D21" s="16"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="21" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="7" t="s">
@@ -972,214 +1051,216 @@
       <c r="C22" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="26" t="s">
+      <c r="D22" s="21" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="27"/>
+      <c r="A23" s="22"/>
       <c r="B23" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="22"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="27"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="7" t="s">
         <v>20</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="22"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="22"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="7" t="s">
         <v>22</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="27"/>
+      <c r="D26" s="22"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="27"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="7" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="27"/>
+      <c r="D27" s="22"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="27"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="7" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="27"/>
+      <c r="D28" s="22"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="27"/>
+      <c r="A29" s="22"/>
       <c r="B29" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="27"/>
+      <c r="D29" s="22"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="28"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="28"/>
+      <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="31" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>1</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="32" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="13"/>
+      <c r="A32" s="31"/>
       <c r="B32" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="D32" s="33"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="13"/>
+      <c r="A33" s="31"/>
       <c r="B33" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="D33" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="D33" s="33"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="8" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" s="16"/>
+        <v>50</v>
+      </c>
+      <c r="D34" s="34"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="30" t="s">
         <v>39</v>
       </c>
       <c r="B35" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D35" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="30" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D36" s="12"/>
+        <v>50</v>
+      </c>
+      <c r="D36" s="30"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D37" s="12"/>
+        <v>50</v>
+      </c>
+      <c r="D37" s="30"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D38" s="12"/>
+        <v>50</v>
+      </c>
+      <c r="D38" s="30"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D39" s="33" t="s">
+      <c r="C39" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" s="17" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="33"/>
-      <c r="B40" s="32" t="s">
+      <c r="A40" s="17"/>
+      <c r="B40" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D40" s="33"/>
+      <c r="C40" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D40" s="17"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="33"/>
-      <c r="B41" s="32" t="s">
+      <c r="A41" s="17"/>
+      <c r="B41" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C41" s="32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" s="33"/>
+      <c r="C41" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D41" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="D39:D41"/>
     <mergeCell ref="A39:A41"/>
     <mergeCell ref="A2:A4"/>
@@ -1194,8 +1275,6 @@
     <mergeCell ref="A35:A38"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="D31:D34"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Edit Index Of Products And Categories
</commit_message>
<xml_diff>
--- a/DigiMovie/INFOs/Permissions.xlsx
+++ b/DigiMovie/INFOs/Permissions.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="55">
   <si>
     <t>Products</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Check in …</t>
   </si>
   <si>
-    <t xml:space="preserve"> action</t>
-  </si>
-  <si>
     <t xml:space="preserve"> view</t>
   </si>
   <si>
@@ -178,6 +175,15 @@
   </si>
   <si>
     <t>[has all roles]</t>
+  </si>
+  <si>
+    <t>AdminIndex</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> مدیر محصولات</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Annonymous </t>
   </si>
 </sst>
 </file>
@@ -352,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -378,85 +384,115 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -746,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,498 +819,469 @@
         <v>29</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="21" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="18"/>
-      <c r="F2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="35" t="s">
+      <c r="D2" s="21"/>
+      <c r="F2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>43</v>
       </c>
+      <c r="J2" s="13" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="19"/>
+      <c r="A3" s="22"/>
       <c r="B3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="F3" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H3" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="J3" s="35" t="s">
-        <v>47</v>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="F3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="20"/>
-      <c r="H4" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="35" t="s">
-        <v>52</v>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="H4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="13" t="s">
-        <v>50</v>
+      <c r="C5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="44"/>
+      <c r="H5" s="12" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="28"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="45"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="28"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="16"/>
+      <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="29"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="41"/>
+    </row>
+    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="28"/>
+      <c r="B13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>31</v>
-      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="42"/>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="29"/>
+      <c r="D14" s="43"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="28"/>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="28"/>
+      <c r="B17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="28"/>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+      <c r="B21" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="18"/>
+      <c r="B22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="19"/>
+      <c r="B23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="24" t="s">
+      <c r="D24" s="24" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" s="25"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="26"/>
-      <c r="B17" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="25"/>
+      <c r="B25" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="25"/>
+      <c r="B26" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="26"/>
+      <c r="D26" s="25"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" s="25"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="25"/>
+      <c r="B28" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="25"/>
+      <c r="B29" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C31" s="25"/>
+      <c r="D31" s="25"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="26"/>
+      <c r="B32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="15"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="15"/>
-      <c r="B20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="15"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
-      <c r="B21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D21" s="16"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="22"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="22"/>
-      <c r="B24" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D24" s="22"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="22"/>
-      <c r="B25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="22"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="22"/>
-      <c r="B26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D26" s="22"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="22"/>
-      <c r="B27" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D27" s="22"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="22"/>
-      <c r="B28" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D28" s="22"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="22"/>
-      <c r="B29" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="22"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="23"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="C33" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="31"/>
-      <c r="B32" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="33"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="31"/>
-      <c r="B33" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" s="33"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="31"/>
       <c r="B34" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
+      <c r="B35" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="33"/>
+      <c r="D35" s="33"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D34" s="34"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="B35" s="11" t="s">
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="30" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="30"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="30"/>
+      <c r="C37" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D37" s="30" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="D38" s="30"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="30"/>
+      <c r="B39" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="36"/>
+      <c r="D39" s="30"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="30"/>
+      <c r="B40" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C38" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="30"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+      <c r="C40" s="37"/>
+      <c r="D40" s="30"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D41" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="B42" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
-      <c r="B40" s="12" t="s">
+      <c r="C42" s="39"/>
+      <c r="D42" s="20"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="20"/>
+      <c r="B43" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C40" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" s="17"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
-      <c r="B41" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" s="17"/>
+      <c r="C43" s="40"/>
+      <c r="D43" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="A39:A41"/>
+  <mergeCells count="29">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="C33:C36"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C16:C19"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="D41:D43"/>
+    <mergeCell ref="A41:A43"/>
     <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A22:A30"/>
-    <mergeCell ref="A11:A17"/>
-    <mergeCell ref="D18:D21"/>
-    <mergeCell ref="D22:D30"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="D20:D23"/>
+    <mergeCell ref="D24:D32"/>
     <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="A35:A38"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="D31:D34"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="A37:A40"/>
+    <mergeCell ref="A33:A36"/>
+    <mergeCell ref="D33:D36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>